<commit_message>
Update Estimation Sample - WBS.xlsx
</commit_message>
<xml_diff>
--- a/Process/Estimation/Estimation Sample - WBS.xlsx
+++ b/Process/Estimation/Estimation Sample - WBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BHN-RAFI\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="578" documentId="8_{26F7CD7B-AE75-4682-AAE2-31C96CAAD7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89723975-D43A-493B-86D2-5D822DA55EAE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D602AF1B-2065-4FA6-A7A1-D1E19CD5E1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{813F1D14-437E-4E9E-A964-A3190BB7C894}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{813F1D14-437E-4E9E-A964-A3190BB7C894}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="87">
   <si>
     <t>S.No</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>MOM</t>
+  </si>
+  <si>
+    <t>Total time</t>
   </si>
 </sst>
 </file>
@@ -4111,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91AC7A6-2934-465A-B104-B8D88A31FA76}">
   <dimension ref="A1:I470"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D14"/>
+    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0">
+      <selection activeCell="F469" sqref="F469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4213,7 +4216,9 @@
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1"/>
@@ -4221,7 +4226,9 @@
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1"/>
@@ -4250,7 +4257,7 @@
       </c>
       <c r="D14" s="2">
         <f>SUM(D2:D12)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -4329,7 +4336,9 @@
       <c r="C23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1"/>
@@ -4353,7 +4362,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2">
         <f>SUM(D15:D25)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4432,7 +4441,9 @@
       <c r="C36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1"/>
@@ -4440,7 +4451,9 @@
       <c r="C37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1"/>
@@ -4456,7 +4469,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2">
         <f>SUM(D28:D38)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -4535,7 +4548,9 @@
       <c r="C49" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1"/>
@@ -4543,7 +4558,9 @@
       <c r="C50" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1"/>
@@ -4559,7 +4576,7 @@
       <c r="C52" s="2"/>
       <c r="D52" s="2">
         <f>SUM(D41:D51)</f>
-        <v>18.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -4638,7 +4655,9 @@
       <c r="C63" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D63" s="1"/>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1"/>
@@ -4646,7 +4665,9 @@
       <c r="C64" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="1"/>
+      <c r="D64" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1"/>
@@ -4662,7 +4683,7 @@
       <c r="C66" s="2"/>
       <c r="D66" s="2">
         <f>SUM(D55:D65)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -4741,7 +4762,9 @@
       <c r="C76" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D76" s="1"/>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1"/>
@@ -4749,7 +4772,9 @@
       <c r="C77" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D77" s="1"/>
+      <c r="D77" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1"/>
@@ -4765,7 +4790,7 @@
       <c r="C79" s="2"/>
       <c r="D79" s="2">
         <f>SUM(D68:D78)</f>
-        <v>19.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -4844,7 +4869,9 @@
       <c r="C89" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D89" s="1"/>
+      <c r="D89" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1"/>
@@ -4852,7 +4879,9 @@
       <c r="C90" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D90" s="1"/>
+      <c r="D90" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1"/>
@@ -4868,7 +4897,7 @@
       <c r="C92" s="2"/>
       <c r="D92" s="2">
         <f>SUM(D81:D91)</f>
-        <v>18.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -4947,7 +4976,9 @@
       <c r="C102" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D102" s="1"/>
+      <c r="D102" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="1"/>
@@ -4955,7 +4986,9 @@
       <c r="C103" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D103" s="1"/>
+      <c r="D103" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="1"/>
@@ -4971,7 +5004,7 @@
       <c r="C105" s="2"/>
       <c r="D105" s="2">
         <f>SUM(D94:D104)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -5050,7 +5083,9 @@
       <c r="C116" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D116" s="1"/>
+      <c r="D116" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1"/>
@@ -5058,7 +5093,9 @@
       <c r="C117" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D117" s="1"/>
+      <c r="D117" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1"/>
@@ -5074,7 +5111,7 @@
       <c r="C119" s="2"/>
       <c r="D119" s="2">
         <f>SUM(D108:D118)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -5153,7 +5190,9 @@
       <c r="C129" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D129" s="1"/>
+      <c r="D129" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="1"/>
@@ -5161,7 +5200,9 @@
       <c r="C130" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D130" s="1"/>
+      <c r="D130" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="1"/>
@@ -5177,7 +5218,7 @@
       <c r="C132" s="2"/>
       <c r="D132" s="2">
         <f>SUM(D121:D131)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -5256,7 +5297,9 @@
       <c r="C142" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D142" s="1"/>
+      <c r="D142" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="1"/>
@@ -5264,7 +5307,9 @@
       <c r="C143" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D143" s="1"/>
+      <c r="D143" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="1"/>
@@ -5280,7 +5325,7 @@
       <c r="C145" s="2"/>
       <c r="D145" s="2">
         <f>SUM(D134:D144)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -5359,7 +5404,9 @@
       <c r="C155" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D155" s="1"/>
+      <c r="D155" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="1"/>
@@ -5367,7 +5414,9 @@
       <c r="C156" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D156" s="1"/>
+      <c r="D156" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="1"/>
@@ -5383,7 +5432,7 @@
       <c r="C158" s="2"/>
       <c r="D158" s="2">
         <f>SUM(D147:D157)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -5462,7 +5511,9 @@
       <c r="C168" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D168" s="1"/>
+      <c r="D168" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="1"/>
@@ -5470,7 +5521,9 @@
       <c r="C169" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D169" s="1"/>
+      <c r="D169" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="1"/>
@@ -5486,7 +5539,7 @@
       <c r="C171" s="2"/>
       <c r="D171" s="2">
         <f>SUM(D160:D170)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -5565,7 +5618,9 @@
       <c r="C181" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D181" s="1"/>
+      <c r="D181" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="1"/>
@@ -5573,7 +5628,9 @@
       <c r="C182" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D182" s="1"/>
+      <c r="D182" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="1"/>
@@ -5589,7 +5646,7 @@
       <c r="C184" s="2"/>
       <c r="D184" s="2">
         <f>SUM(D173:D183)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -5668,7 +5725,9 @@
       <c r="C194" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D194" s="1"/>
+      <c r="D194" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" s="1"/>
@@ -5676,7 +5735,9 @@
       <c r="C195" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D195" s="1"/>
+      <c r="D195" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="1"/>
@@ -5692,7 +5753,7 @@
       <c r="C197" s="2"/>
       <c r="D197" s="2">
         <f>SUM(D186:D196)</f>
-        <v>18.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -5771,7 +5832,9 @@
       <c r="C207" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D207" s="1"/>
+      <c r="D207" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="1"/>
@@ -5779,7 +5842,9 @@
       <c r="C208" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D208" s="1"/>
+      <c r="D208" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="1"/>
@@ -5795,7 +5860,7 @@
       <c r="C210" s="2"/>
       <c r="D210" s="2">
         <f>SUM(D199:D209)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -5874,7 +5939,9 @@
       <c r="C220" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D220" s="1"/>
+      <c r="D220" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="1"/>
@@ -5882,7 +5949,9 @@
       <c r="C221" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D221" s="1"/>
+      <c r="D221" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="222" spans="1:4">
       <c r="A222" s="1"/>
@@ -5898,7 +5967,7 @@
       <c r="C223" s="2"/>
       <c r="D223" s="2">
         <f>SUM(D212:D222)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -5977,7 +6046,9 @@
       <c r="C233" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D233" s="1"/>
+      <c r="D233" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="234" spans="1:4">
       <c r="A234" s="1"/>
@@ -5993,7 +6064,9 @@
       <c r="C235" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D235" s="1"/>
+      <c r="D235" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="236" spans="1:4">
       <c r="A236" s="2"/>
@@ -6001,7 +6074,7 @@
       <c r="C236" s="2"/>
       <c r="D236" s="2">
         <f>SUM(D225:D235)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -6080,7 +6153,9 @@
       <c r="C246" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D246" s="1"/>
+      <c r="D246" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="247" spans="1:4">
       <c r="A247" s="1"/>
@@ -6088,7 +6163,9 @@
       <c r="C247" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D247" s="1"/>
+      <c r="D247" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="248" spans="1:4">
       <c r="A248" s="1"/>
@@ -6104,7 +6181,7 @@
       <c r="C249" s="2"/>
       <c r="D249" s="2">
         <f>SUM(D238:D248)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -6183,7 +6260,9 @@
       <c r="C259" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D259" s="1"/>
+      <c r="D259" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="260" spans="1:4">
       <c r="A260" s="1"/>
@@ -6191,7 +6270,9 @@
       <c r="C260" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D260" s="1"/>
+      <c r="D260" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="1"/>
@@ -6207,7 +6288,7 @@
       <c r="C262" s="2"/>
       <c r="D262" s="2">
         <f>SUM(D251:D261)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -6286,7 +6367,9 @@
       <c r="C272" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D272" s="1"/>
+      <c r="D272" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="273" spans="1:4">
       <c r="A273" s="1"/>
@@ -6294,7 +6377,9 @@
       <c r="C273" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D273" s="1"/>
+      <c r="D273" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="274" spans="1:4">
       <c r="A274" s="1"/>
@@ -6310,7 +6395,7 @@
       <c r="C275" s="2"/>
       <c r="D275" s="2">
         <f>SUM(D264:D274)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -6389,7 +6474,9 @@
       <c r="C285" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D285" s="1"/>
+      <c r="D285" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="286" spans="1:4">
       <c r="A286" s="1"/>
@@ -6397,7 +6484,9 @@
       <c r="C286" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D286" s="1"/>
+      <c r="D286" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="287" spans="1:4">
       <c r="A287" s="1"/>
@@ -6413,7 +6502,7 @@
       <c r="C288" s="2"/>
       <c r="D288" s="2">
         <f>SUM(D277:D287)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -6492,7 +6581,9 @@
       <c r="C298" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D298" s="1"/>
+      <c r="D298" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="299" spans="1:4">
       <c r="A299" s="1"/>
@@ -6500,7 +6591,9 @@
       <c r="C299" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D299" s="1"/>
+      <c r="D299" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="1"/>
@@ -6516,7 +6609,7 @@
       <c r="C301" s="2"/>
       <c r="D301" s="2">
         <f>SUM(D290:D300)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -6595,7 +6688,9 @@
       <c r="C311" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D311" s="1"/>
+      <c r="D311" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="312" spans="1:4">
       <c r="A312" s="1"/>
@@ -6603,7 +6698,9 @@
       <c r="C312" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D312" s="1"/>
+      <c r="D312" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="313" spans="1:4">
       <c r="A313" s="1"/>
@@ -6619,7 +6716,7 @@
       <c r="C314" s="2"/>
       <c r="D314" s="2">
         <f>SUM(D303:D313)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -6698,7 +6795,9 @@
       <c r="C324" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D324" s="1"/>
+      <c r="D324" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="325" spans="1:4">
       <c r="A325" s="1"/>
@@ -6706,7 +6805,9 @@
       <c r="C325" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D325" s="1"/>
+      <c r="D325" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="326" spans="1:4">
       <c r="A326" s="1"/>
@@ -6722,7 +6823,7 @@
       <c r="C327" s="2"/>
       <c r="D327" s="2">
         <f>SUM(D316:D326)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -6801,7 +6902,9 @@
       <c r="C337" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D337" s="1"/>
+      <c r="D337" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="338" spans="1:4">
       <c r="A338" s="1"/>
@@ -6809,7 +6912,9 @@
       <c r="C338" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D338" s="1"/>
+      <c r="D338" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="339" spans="1:4">
       <c r="A339" s="1"/>
@@ -6825,7 +6930,7 @@
       <c r="C340" s="2"/>
       <c r="D340" s="2">
         <f>SUM(D329:D339)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -6904,7 +7009,9 @@
       <c r="C350" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D350" s="1"/>
+      <c r="D350" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="351" spans="1:4">
       <c r="A351" s="1"/>
@@ -6912,7 +7019,9 @@
       <c r="C351" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D351" s="1"/>
+      <c r="D351" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="352" spans="1:4">
       <c r="A352" s="1"/>
@@ -6928,7 +7037,7 @@
       <c r="C353" s="2"/>
       <c r="D353" s="2">
         <f>SUM(D342:D352)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -7007,7 +7116,9 @@
       <c r="C363" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D363" s="1"/>
+      <c r="D363" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="364" spans="1:4">
       <c r="A364" s="1"/>
@@ -7015,7 +7126,9 @@
       <c r="C364" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D364" s="1"/>
+      <c r="D364" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="365" spans="1:4">
       <c r="A365" s="1"/>
@@ -7031,7 +7144,7 @@
       <c r="C366" s="2"/>
       <c r="D366" s="2">
         <f>SUM(D355:D365)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -7110,7 +7223,9 @@
       <c r="C376" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D376" s="1"/>
+      <c r="D376" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="377" spans="1:4">
       <c r="A377" s="1"/>
@@ -7118,7 +7233,9 @@
       <c r="C377" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D377" s="1"/>
+      <c r="D377" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="378" spans="1:4">
       <c r="A378" s="1"/>
@@ -7134,7 +7251,7 @@
       <c r="C379" s="2"/>
       <c r="D379" s="2">
         <f>SUM(D368:D378)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7213,7 +7330,9 @@
       <c r="C389" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D389" s="1"/>
+      <c r="D389" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="390" spans="1:4">
       <c r="A390" s="1"/>
@@ -7221,7 +7340,9 @@
       <c r="C390" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D390" s="1"/>
+      <c r="D390" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="391" spans="1:4">
       <c r="A391" s="1"/>
@@ -7237,7 +7358,7 @@
       <c r="C392" s="2"/>
       <c r="D392" s="2">
         <f>SUM(D381:D391)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -7316,7 +7437,9 @@
       <c r="C402" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D402" s="1"/>
+      <c r="D402" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="403" spans="1:4">
       <c r="A403" s="1"/>
@@ -7324,7 +7447,9 @@
       <c r="C403" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D403" s="1"/>
+      <c r="D403" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="404" spans="1:4">
       <c r="A404" s="1"/>
@@ -7340,7 +7465,7 @@
       <c r="C405" s="2"/>
       <c r="D405" s="2">
         <f>SUM(D394:D404)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -7419,7 +7544,9 @@
       <c r="C415" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D415" s="1"/>
+      <c r="D415" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="416" spans="1:4">
       <c r="A416" s="1"/>
@@ -7427,7 +7554,9 @@
       <c r="C416" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D416" s="1"/>
+      <c r="D416" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="417" spans="1:4">
       <c r="A417" s="1"/>
@@ -7443,7 +7572,7 @@
       <c r="C418" s="2"/>
       <c r="D418" s="2">
         <f>SUM(D407:D417)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="420" spans="1:4">
@@ -7522,7 +7651,9 @@
       <c r="C428" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D428" s="1"/>
+      <c r="D428" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="429" spans="1:4">
       <c r="A429" s="1"/>
@@ -7530,7 +7661,9 @@
       <c r="C429" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D429" s="1"/>
+      <c r="D429" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="430" spans="1:4">
       <c r="A430" s="1"/>
@@ -7546,7 +7679,7 @@
       <c r="C431" s="2"/>
       <c r="D431" s="2">
         <f>SUM(D420:D430)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="433" spans="1:4">
@@ -7625,7 +7758,9 @@
       <c r="C441" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D441" s="1"/>
+      <c r="D441" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="442" spans="1:4">
       <c r="A442" s="1"/>
@@ -7633,7 +7768,9 @@
       <c r="C442" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D442" s="1"/>
+      <c r="D442" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="443" spans="1:4">
       <c r="A443" s="1"/>
@@ -7649,7 +7786,7 @@
       <c r="C444" s="2"/>
       <c r="D444" s="2">
         <f>SUM(D433:D443)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -7728,7 +7865,9 @@
       <c r="C454" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D454" s="1"/>
+      <c r="D454" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="455" spans="1:4">
       <c r="A455" s="1"/>
@@ -7736,7 +7875,9 @@
       <c r="C455" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D455" s="1"/>
+      <c r="D455" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="456" spans="1:4">
       <c r="A456" s="1"/>
@@ -7752,7 +7893,7 @@
       <c r="C457" s="2"/>
       <c r="D457" s="2">
         <f>SUM(D446:D456)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="459" spans="1:4">
@@ -7831,7 +7972,9 @@
       <c r="C467" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D467" s="1"/>
+      <c r="D467" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="468" spans="1:4">
       <c r="A468" s="1"/>
@@ -7839,7 +7982,9 @@
       <c r="C468" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D468" s="1"/>
+      <c r="D468" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="469" spans="1:4">
       <c r="A469" s="1"/>
@@ -7855,7 +8000,7 @@
       <c r="C470" s="2"/>
       <c r="D470" s="2">
         <f>SUM(D459:D469)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -7865,10 +8010,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE0C87E-44F3-4CBC-941A-A0ED96B6110E}">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="G145" sqref="G145"/>
+    <sheetView topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7911,7 +8056,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -7919,7 +8064,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -7927,7 +8072,7 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -7935,7 +8080,7 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -7943,7 +8088,7 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -7951,7 +8096,7 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8000,7 +8145,7 @@
       </c>
       <c r="D14" s="2">
         <f>SUM(D2:D12)</f>
-        <v>19</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -8464,7 +8609,7 @@
         <v>6</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -8472,7 +8617,7 @@
         <v>8</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -8561,7 +8706,7 @@
       </c>
       <c r="D89" s="2">
         <f>SUM(D77:D87)</f>
-        <v>20.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -8694,7 +8839,7 @@
         <v>8</v>
       </c>
       <c r="D108">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -8702,7 +8847,7 @@
         <v>10</v>
       </c>
       <c r="D109">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -8710,7 +8855,7 @@
         <v>12</v>
       </c>
       <c r="D110">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -8718,7 +8863,7 @@
         <v>13</v>
       </c>
       <c r="D111">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -8726,7 +8871,7 @@
         <v>14</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -8734,7 +8879,7 @@
         <v>15</v>
       </c>
       <c r="D113">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -8742,7 +8887,7 @@
         <v>16</v>
       </c>
       <c r="D114">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -8783,7 +8928,7 @@
       </c>
       <c r="D119" s="2">
         <f>SUM(D107:D117)</f>
-        <v>19</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -8805,7 +8950,7 @@
         <v>8</v>
       </c>
       <c r="D123">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -8821,7 +8966,7 @@
         <v>12</v>
       </c>
       <c r="D125">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -8845,7 +8990,7 @@
         <v>15</v>
       </c>
       <c r="D128">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -8894,7 +9039,7 @@
       </c>
       <c r="D134" s="2">
         <f>SUM(D122:D132)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -9119,6 +9264,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="167" spans="1:4">
+      <c r="C167" t="s">
+        <v>86</v>
+      </c>
+      <c r="D167">
+        <v>252.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>